<commit_message>
Added buttons, scene setup
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Arcade_Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40BB38D2-9D9A-4097-9B69-E94D48AD4F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D38756-14F7-447D-B93E-7BDB7551543D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C2F40B01-6141-4C70-A466-5B0B19B001FE}"/>
   </bookViews>
@@ -125,12 +125,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -145,8 +151,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -463,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF1BD46-C8AE-4161-A441-EF4123DCA11C}">
   <dimension ref="B1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,17 +505,17 @@
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -528,17 +535,17 @@
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -558,7 +565,7 @@
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -573,7 +580,7 @@
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -583,17 +590,17 @@
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -608,7 +615,7 @@
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>